<commit_message>
worked on export issue
</commit_message>
<xml_diff>
--- a/Presentation/Diyan.API/FormatFiles/Template_Territories.xlsx
+++ b/Presentation/Diyan.API/FormatFiles/Template_Territories.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Sujay-Git\Diyan_API\Presentation\Diyan.API\FormatFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3F49B5-43B9-4A27-B8E6-332B5BF62DED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,30 +25,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>IsActive</t>
   </si>
   <si>
-    <t>CityName</t>
-  </si>
-  <si>
-    <t>RegionName</t>
-  </si>
-  <si>
     <t>StateName</t>
   </si>
   <si>
     <t>DistrictName</t>
   </si>
   <si>
-    <t>CityGrade</t>
+    <t>India</t>
+  </si>
+  <si>
+    <t>CountryName</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>Bihar</t>
+  </si>
+  <si>
+    <t>Patna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,52 +402,72 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>